<commit_message>
refactorizacion nombre clase (por problema de comatibilidad entre versiones de php)
</commit_message>
<xml_diff>
--- a/public/week_data.xlsx
+++ b/public/week_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
   <si>
     <t>USUARIO ORLANDO BEJARANO FERNANDEZ</t>
   </si>
@@ -266,12 +266,12 @@
     <t>2022-10-15</t>
   </si>
   <si>
+    <t>MARISOL DANIELA RAMOS</t>
+  </si>
+  <si>
     <t>2022-10-17</t>
   </si>
   <si>
-    <t>MARISOL DANIELA RAMOS</t>
-  </si>
-  <si>
     <t>2022-10-18</t>
   </si>
   <si>
@@ -335,13 +335,34 @@
     <t>2022-12-05</t>
   </si>
   <si>
+    <t>2022-12-12</t>
+  </si>
+  <si>
     <t>JUANA ESTHER MICHEL CRUZ</t>
   </si>
   <si>
-    <t>2022-12-12</t>
-  </si>
-  <si>
     <t>2022-12-13</t>
+  </si>
+  <si>
+    <t>2022-12-19</t>
+  </si>
+  <si>
+    <t>JUANA ANGELICA MENDIETA CARDONA</t>
+  </si>
+  <si>
+    <t>2022-12-21</t>
+  </si>
+  <si>
+    <t>LIMBER RAYNARD GARNICA MEZZA</t>
+  </si>
+  <si>
+    <t>2022-12-22</t>
+  </si>
+  <si>
+    <t>LISELDA MILENIA ROMERO ALARCON</t>
+  </si>
+  <si>
+    <t>MARCO ANTONIO COLODRO</t>
   </si>
   <si>
     <t xml:space="preserve">FILTRO: </t>
@@ -792,10 +813,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N112"/>
+  <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B112" sqref="B112"/>
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -832,14 +853,14 @@
         <v>7</v>
       </c>
       <c r="K6" s="4">
-        <v>74013.86</v>
+        <v>76343.96</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4">
-        <v>2330.1</v>
+        <v>8952.1</v>
       </c>
       <c r="N6" s="4">
-        <v>76343.96</v>
+        <v>85296.06</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1294,10 +1315,10 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="4">
-        <v>5784526</v>
+        <v>7217197</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1312,7 +1333,7 @@
         <v>7</v>
       </c>
       <c r="K23" s="4">
-        <v>498.1</v>
+        <v>950.0</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>31</v>
@@ -1324,10 +1345,10 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="4">
-        <v>7217197</v>
+        <v>5784526</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1342,7 +1363,7 @@
         <v>7</v>
       </c>
       <c r="K24" s="4">
-        <v>950.0</v>
+        <v>498.1</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>31</v>
@@ -2224,10 +2245,10 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="4">
-        <v>7143371</v>
+        <v>5787275</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2242,7 +2263,7 @@
         <v>7</v>
       </c>
       <c r="K54" s="4">
-        <v>287.47</v>
+        <v>1010.6</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>62</v>
@@ -2254,10 +2275,10 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="4">
-        <v>5787275</v>
+        <v>7143371</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2272,7 +2293,7 @@
         <v>7</v>
       </c>
       <c r="K55" s="4">
-        <v>1010.6</v>
+        <v>287.47</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>62</v>
@@ -2584,10 +2605,10 @@
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="4">
-        <v>7254095</v>
+        <v>7143371</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -2602,7 +2623,7 @@
         <v>7</v>
       </c>
       <c r="K66" s="4">
-        <v>185.1</v>
+        <v>287.47</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>76</v>
@@ -2614,10 +2635,10 @@
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="4">
-        <v>7143371</v>
+        <v>7254095</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -2632,7 +2653,7 @@
         <v>7</v>
       </c>
       <c r="K67" s="4">
-        <v>287.47</v>
+        <v>185.1</v>
       </c>
       <c r="L67" s="5" t="s">
         <v>76</v>
@@ -2824,10 +2845,10 @@
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -2842,10 +2863,10 @@
         <v>7</v>
       </c>
       <c r="K74" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M74" s="4"/>
       <c r="N74" s="6" t="s">
@@ -2854,10 +2875,10 @@
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -2872,10 +2893,10 @@
         <v>7</v>
       </c>
       <c r="K75" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L75" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M75" s="4"/>
       <c r="N75" s="6" t="s">
@@ -2884,10 +2905,10 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="4">
-        <v>7143371</v>
+        <v>1899092</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -2902,7 +2923,7 @@
         <v>7</v>
       </c>
       <c r="K76" s="4">
-        <v>287.47</v>
+        <v>770.0</v>
       </c>
       <c r="L76" s="5" t="s">
         <v>85</v>
@@ -2914,10 +2935,10 @@
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="4">
-        <v>1899092</v>
+        <v>7143371</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -2932,7 +2953,7 @@
         <v>7</v>
       </c>
       <c r="K77" s="4">
-        <v>770.0</v>
+        <v>287.47</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>85</v>
@@ -3004,10 +3025,10 @@
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3022,7 +3043,7 @@
         <v>7</v>
       </c>
       <c r="K80" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>88</v>
@@ -3034,10 +3055,10 @@
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -3052,7 +3073,7 @@
         <v>7</v>
       </c>
       <c r="K81" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>88</v>
@@ -3154,10 +3175,10 @@
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="4">
-        <v>7259089</v>
+        <v>1899092</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -3172,7 +3193,7 @@
         <v>7</v>
       </c>
       <c r="K85" s="4">
-        <v>818.38</v>
+        <v>770.0</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>91</v>
@@ -3184,10 +3205,10 @@
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -3202,7 +3223,7 @@
         <v>7</v>
       </c>
       <c r="K86" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>91</v>
@@ -3214,10 +3235,10 @@
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="4">
-        <v>1899092</v>
+        <v>7254095</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
@@ -3232,7 +3253,7 @@
         <v>7</v>
       </c>
       <c r="K87" s="4">
-        <v>770.0</v>
+        <v>185.1</v>
       </c>
       <c r="L87" s="5" t="s">
         <v>91</v>
@@ -3304,10 +3325,10 @@
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
@@ -3322,7 +3343,7 @@
         <v>7</v>
       </c>
       <c r="K90" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L90" s="5" t="s">
         <v>95</v>
@@ -3334,10 +3355,10 @@
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
@@ -3352,7 +3373,7 @@
         <v>7</v>
       </c>
       <c r="K91" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>95</v>
@@ -3397,7 +3418,7 @@
         <v>7259089</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -3454,10 +3475,10 @@
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="4">
-        <v>1899092</v>
+        <v>5684823</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
@@ -3472,7 +3493,7 @@
         <v>7</v>
       </c>
       <c r="K95" s="4">
-        <v>770.0</v>
+        <v>665.0</v>
       </c>
       <c r="L95" s="5" t="s">
         <v>98</v>
@@ -3484,10 +3505,10 @@
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="4">
-        <v>5684823</v>
+        <v>1899092</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -3502,7 +3523,7 @@
         <v>7</v>
       </c>
       <c r="K96" s="4">
-        <v>665.0</v>
+        <v>770.0</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>98</v>
@@ -3574,10 +3595,10 @@
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -3592,7 +3613,7 @@
         <v>7</v>
       </c>
       <c r="K99" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>101</v>
@@ -3604,10 +3625,10 @@
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -3622,7 +3643,7 @@
         <v>7</v>
       </c>
       <c r="K100" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L100" s="5" t="s">
         <v>101</v>
@@ -3697,7 +3718,7 @@
         <v>7259089</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -3784,10 +3805,10 @@
     </row>
     <row r="106" spans="1:14">
       <c r="A106" s="4">
-        <v>7254095</v>
+        <v>7259089</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -3802,7 +3823,7 @@
         <v>7</v>
       </c>
       <c r="K106" s="4">
-        <v>185.1</v>
+        <v>818.38</v>
       </c>
       <c r="L106" s="5" t="s">
         <v>105</v>
@@ -3814,10 +3835,10 @@
     </row>
     <row r="107" spans="1:14">
       <c r="A107" s="4">
-        <v>7259089</v>
+        <v>7254095</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -3832,7 +3853,7 @@
         <v>7</v>
       </c>
       <c r="K107" s="4">
-        <v>818.38</v>
+        <v>185.1</v>
       </c>
       <c r="L107" s="5" t="s">
         <v>105</v>
@@ -3844,10 +3865,10 @@
     </row>
     <row r="108" spans="1:14">
       <c r="A108" s="4">
-        <v>7103441</v>
+        <v>7254095</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -3862,22 +3883,22 @@
         <v>7</v>
       </c>
       <c r="K108" s="4">
-        <v>1480.0</v>
+        <v>185.1</v>
       </c>
       <c r="L108" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M108" s="4"/>
-      <c r="N108" s="7" t="s">
-        <v>5</v>
+      <c r="N108" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:14">
       <c r="A109" s="4">
-        <v>7254095</v>
+        <v>7103441</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -3892,14 +3913,14 @@
         <v>7</v>
       </c>
       <c r="K109" s="4">
-        <v>185.1</v>
+        <v>1480.0</v>
       </c>
       <c r="L109" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M109" s="4"/>
-      <c r="N109" s="7" t="s">
-        <v>5</v>
+      <c r="N109" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:14">
@@ -3928,15 +3949,165 @@
         <v>108</v>
       </c>
       <c r="M110" s="4"/>
-      <c r="N110" s="7" t="s">
+      <c r="N110" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="A111" s="4">
+        <v>7254095</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K111" s="4">
+        <v>185.1</v>
+      </c>
+      <c r="L111" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M111" s="4"/>
+      <c r="N111" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:14">
-      <c r="A112" t="s">
-        <v>109</v>
-      </c>
-      <c r="B112" t="s">
+      <c r="A112" s="4">
+        <v>5032867</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K112" s="4">
+        <v>390.0</v>
+      </c>
+      <c r="L112" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M112" s="4"/>
+      <c r="N112" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="A113" s="4">
+        <v>5797560</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K113" s="4">
+        <v>320.0</v>
+      </c>
+      <c r="L113" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M113" s="4"/>
+      <c r="N113" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="4">
+        <v>7247912</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K114" s="4">
+        <v>8000.0</v>
+      </c>
+      <c r="L114" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M114" s="4"/>
+      <c r="N114" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="A115" s="4">
+        <v>7190526</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K115" s="4">
+        <v>57.0</v>
+      </c>
+      <c r="L115" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M115" s="4"/>
+      <c r="N115" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4254,13 +4425,28 @@
     <mergeCell ref="B110:E110"/>
     <mergeCell ref="F110:I110"/>
     <mergeCell ref="L110:M110"/>
-    <mergeCell ref="B112:N112"/>
+    <mergeCell ref="B111:E111"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="L111:M111"/>
+    <mergeCell ref="B112:E112"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="L112:M112"/>
+    <mergeCell ref="B113:E113"/>
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="L113:M113"/>
+    <mergeCell ref="B114:E114"/>
+    <mergeCell ref="F114:I114"/>
+    <mergeCell ref="L114:M114"/>
+    <mergeCell ref="B115:E115"/>
+    <mergeCell ref="F115:I115"/>
+    <mergeCell ref="L115:M115"/>
+    <mergeCell ref="B117:N117"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="73" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader>&amp;L2022-12-07 06:01:19&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
+    <oddHeader>&amp;L2022-12-15 10:47:17&amp;C&amp;HECOMSOFT&amp;RDR. ORLANDO BEJARANO FERNANDEZ</oddHeader>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>